<commit_message>
refactor: Improve Excel schema format and simplify schema statistics
- Rename column_type to data_type in Excel schema for consistency
- Add is_nullable column to Excel schema with YES/NO values
- Update schema ingestion to read is_nullable from Excel files
- Simplify schema statistics to only include total_tables
- Update Excel parser to validate and parse new columns
- Update create_data_postgres.py to apply NOT NULL constraints
- Update documentation with new Excel format requirements

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/schema_files/load_balancer_schema.xlsx
+++ b/schema_files/load_balancer_schema.xlsx
@@ -56,9 +56,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -426,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,15 +450,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>column_type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+          <t>data_type</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>is_nullable</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>table_description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>column_description</t>
         </is>
@@ -479,10 +487,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Unique load balancer identifier</t>
         </is>
@@ -506,10 +519,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Load balancer name</t>
         </is>
@@ -533,10 +551,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Management IP address of the load balancer</t>
         </is>
@@ -560,10 +583,15 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Current operational status (active, inactive, maintenance)</t>
         </is>
@@ -587,10 +615,15 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Datacenter location where load balancer is deployed</t>
         </is>
@@ -614,10 +647,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Load balancer instances managing traffic distribution</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>When the load balancer was created</t>
         </is>
@@ -641,10 +679,15 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Unique virtual IP identifier</t>
         </is>
@@ -668,10 +711,15 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Virtual IP address exposed to clients</t>
         </is>
@@ -695,10 +743,15 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Port number for the service</t>
         </is>
@@ -722,10 +775,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Protocol used (HTTP, HTTPS, TCP, UDP)</t>
         </is>
@@ -749,10 +807,15 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Load balancer handling this VIP</t>
         </is>
@@ -776,10 +839,15 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Backend server pool name</t>
         </is>
@@ -803,10 +871,15 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>URL for health check monitoring</t>
         </is>
@@ -830,10 +903,15 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Virtual IP addresses for application access</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>When the VIP was created</t>
         </is>
@@ -857,10 +935,15 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Unique wide IP identifier</t>
         </is>
@@ -884,10 +967,15 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>DNS domain name for the wide IP</t>
         </is>
@@ -911,10 +999,15 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Load balancing algorithm (round-robin, geo, ratio)</t>
         </is>
@@ -938,10 +1031,15 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>DNS Time-to-Live in seconds</t>
         </is>
@@ -965,10 +1063,15 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>Current operational status (enabled, disabled)</t>
         </is>
@@ -992,10 +1095,15 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>Global server load balancing DNS entries</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>When the wide IP was created</t>
         </is>
@@ -1019,10 +1127,15 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Unique pool assignment identifier</t>
         </is>
@@ -1046,10 +1159,15 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Wide IP this pool belongs to</t>
         </is>
@@ -1073,10 +1191,15 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Virtual IP in this pool</t>
         </is>
@@ -1100,10 +1223,15 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Priority order for traffic distribution</t>
         </is>
@@ -1127,10 +1255,15 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Traffic ratio weight for this VIP</t>
         </is>
@@ -1154,10 +1287,15 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>Pools of virtual IPs assigned to wide IPs</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Whether this pool member is active</t>
         </is>
@@ -1181,10 +1319,15 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Unique backend server identifier</t>
         </is>
@@ -1208,10 +1351,15 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Server hostname</t>
         </is>
@@ -1235,10 +1383,15 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Server IP address</t>
         </is>
@@ -1262,10 +1415,15 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>Service port number</t>
         </is>
@@ -1289,10 +1447,15 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Pool this server belongs to</t>
         </is>
@@ -1316,10 +1479,15 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Load balancer managing this server</t>
         </is>
@@ -1343,10 +1511,15 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Current health check status (up, down, unknown)</t>
         </is>
@@ -1370,10 +1543,15 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>Physical servers handling actual traffic</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Datacenter location</t>
         </is>
@@ -1397,10 +1575,15 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>Unique stat record identifier</t>
         </is>
@@ -1424,10 +1607,15 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>Virtual IP these stats belong to</t>
         </is>
@@ -1451,10 +1639,15 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>When the stats were recorded</t>
         </is>
@@ -1478,10 +1671,15 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>Number of requests per second</t>
         </is>
@@ -1505,10 +1703,15 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>Bytes received</t>
         </is>
@@ -1532,10 +1735,15 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>Bytes sent</t>
         </is>
@@ -1559,10 +1767,15 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>Traffic statistics and metrics</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>Number of active connections</t>
         </is>

</xml_diff>